<commit_message>
Added OnlineNotesService.rar REST Implementation and Upadted  Tasks xls
</commit_message>
<xml_diff>
--- a/Project Requirements/Tasks.xlsx
+++ b/Project Requirements/Tasks.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="REST SERVICES" sheetId="2" r:id="rId2"/>
+    <sheet name="OnlineNotes REST Service" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Hibernate Implementation with trasnsaction</t>
   </si>
@@ -57,15 +57,6 @@
     <t>Notpad Application separate UI and Service</t>
   </si>
   <si>
-    <t>Load file from file system</t>
-  </si>
-  <si>
-    <t>Create Folder local</t>
-  </si>
-  <si>
-    <t>Move folder  to git repository</t>
-  </si>
-  <si>
     <t>How to configure mutiple properties files in Spring</t>
   </si>
   <si>
@@ -81,20 +72,237 @@
     <t>SpringTasks.rar</t>
   </si>
   <si>
-    <t>Start Time-End Time</t>
-  </si>
-  <si>
     <t>Creation and management of local repository and files/folders and updating TASKS list and uploading to Remote repository.</t>
   </si>
   <si>
     <t>09:20 AM - 10-40 AM(1hr 20 min)</t>
+  </si>
+  <si>
+    <t>S#</t>
+  </si>
+  <si>
+    <t>OPERATION</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>REQUEST CONTENT TYPE</t>
+  </si>
+  <si>
+    <t>RESPONSE CONTENT TYPE</t>
+  </si>
+  <si>
+    <t>REQUEST BODY</t>
+  </si>
+  <si>
+    <t>RESPONSE BODY</t>
+  </si>
+  <si>
+    <t>METHOD TYPE</t>
+  </si>
+  <si>
+    <t>Create User</t>
+  </si>
+  <si>
+    <t>/create</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {
+     "FIRST NAME": "JOHN",
+     "LAST NAME":" A"
+     "ADDRESS": {
+       "STREET 1":" ",
+    "STREET 2":" "
+     }
+     }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   "STATUS":"USER CREATED SUCCESSFULLY",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "ID":"101"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>Create Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{      
+id:null,       
+name: "Note From REST",      
+type: ".txt",      
+content: "Added note from rest client",      
+createdDate: null,      
+updatedDate: null,      
+status: "Active",      
+location: null,      
+folder:{      
+ "id"":1      
+ },      
+user:{      
+ "id":1      
+ },      
+searchString: null      
+}      
+</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/create/</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Created Note Successfully !</t>
+  </si>
+  <si>
+    <t>Update Note</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/list/</t>
+  </si>
+  <si>
+    <t>Get All Notes</t>
+  </si>
+  <si>
+    <t>[{
+    "id": 13,
+    "name": "Notes",
+    "type": ".txt",
+    "content": "Content",
+    "createdDate": null,
+    "updatedDate": null,
+    "status": "Active",
+    "location": null,
+    "folder": null,
+    "user": null,
+    "searchString": null
+  },
+  {
+    "id": 14,
+    "name": "Java Notes",
+    "type": ".txt",
+    "content": "Polymorphism\r\nEncapsulation\r\nAbstraction\r\nInheritance\r\n",
+    "createdDate": null,
+    "updatedDate": null,
+    "status": "Active",
+    "location": null,
+    "folder": null,
+    "user": null,
+    "searchString": null
+  }]</t>
+  </si>
+  <si>
+    <t>Get Notes By Id</t>
+  </si>
+  <si>
+    <t>/list/{id}</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>/list/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"id": 15
+"name": "Note From REST"
+"type": ".txt"
+"content": "Added note from rest client"
+"createdDate": null
+"updatedDate": null
+"status": "Active"
+"location": null
+"folder": null
+"user": null
+"searchString": null
+}
+</t>
+  </si>
+  <si>
+    <t>Delete Notes</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>/delete/{id}</t>
+  </si>
+  <si>
+    <t>/delete/16</t>
+  </si>
+  <si>
+    <t>Deleted Note Successfully !</t>
+  </si>
+  <si>
+    <t>Notes updated Successfully !</t>
+  </si>
+  <si>
+    <t>/create/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+"id": 1,
+"name": "Sample CV",
+"type": ".txt",
+"content": "UPDATED UPDATED",
+"createdDate": null,
+"updatedDate": null,
+"status": "Active",
+"location": null,
+"folder": {
+ "id":1
+ },
+"user": {
+ "id":1
+ },
+"searchString": null
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)OnlineNotesService - REST Service </t>
+  </si>
+  <si>
+    <t>2)OnlineNotesUI</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>2 HRS</t>
+  </si>
+  <si>
+    <t>3  HRS</t>
+  </si>
+  <si>
+    <t>OnlineNotesService Implemented using Spring REST 4.1.2 version. Do I need to implement again?</t>
+  </si>
+  <si>
+    <t>Added application on git ,OnlineNotesService.rar in Implementations directory.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +314,21 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,6 +370,18 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -478,19 +713,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.85546875" style="4" customWidth="1"/>
     <col min="2" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="26" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -503,55 +738,55 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
         <v>42643</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
         <v>42643</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42643</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2">
-        <v>42643</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>42647</v>
@@ -559,128 +794,153 @@
       <c r="C7" s="2">
         <v>42647</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
         <v>42647</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="B12" s="2">
+        <v>42647</v>
+      </c>
+      <c r="C12" s="2">
+        <v>42647</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="2">
+        <v>42647</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B13" s="2">
+        <v>42648</v>
+      </c>
       <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2">
-        <v>42647</v>
+        <v>42648</v>
       </c>
       <c r="C17" s="2">
-        <v>42647</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
-        <v>42647</v>
-      </c>
-      <c r="C18" s="2">
         <v>42648</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="D17" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2">
-        <v>42647</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B19" s="2">
         <v>42648</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="C19" s="2">
+        <v>42648</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B21" s="2">
         <v>42648</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C21" s="2">
         <v>42648</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="D21" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B23" s="2">
         <v>42648</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C23" s="2">
         <v>42648</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="D23" s="8"/>
+      <c r="F23" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B25" s="2">
         <v>42648</v>
       </c>
-      <c r="C26" s="2">
-        <v>42648</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2">
+        <v>42649</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="2">
-        <v>42648</v>
-      </c>
-      <c r="C28" s="2">
-        <v>42649</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -692,24 +952,254 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="285" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="285" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add OrderServices and schemas
</commit_message>
<xml_diff>
--- a/Project Requirements/Tasks.xlsx
+++ b/Project Requirements/Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="9555" windowHeight="5190"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="9555" windowHeight="5130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>Hibernate Implementation with trasnsaction</t>
   </si>
@@ -296,6 +296,18 @@
   </si>
   <si>
     <t>Added application on git ,OnlineNotesService.rar in Implementations directory.</t>
+  </si>
+  <si>
+    <t>jersey.config.server.provider.packages</t>
+  </si>
+  <si>
+    <t>Started and completed  10/07/2016 - One hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Creating Login page for note pad application and add roles in db and add descriptor</t>
   </si>
 </sst>
 </file>
@@ -713,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +737,7 @@
     <col min="2" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="26" style="4" customWidth="1"/>
+    <col min="6" max="6" width="44.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -875,8 +887,14 @@
       <c r="D17" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <v>42648</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
@@ -888,6 +906,12 @@
       </c>
       <c r="D19" s="8" t="s">
         <v>64</v>
+      </c>
+      <c r="E19" s="2">
+        <v>42650</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -942,6 +966,16 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>